<commit_message>
Added loading and some quality of life changes. Weird error though with processing only one customer code, but doing all the emails and products entered
</commit_message>
<xml_diff>
--- a/AutoBlueSystemSrc/customer_product_codes/PICCTH.xlsx
+++ b/AutoBlueSystemSrc/customer_product_codes/PICCTH.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -626,6 +626,19 @@
       </c>
       <c r="C15" t="inlineStr"/>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>add id	fresh egg rigatoni (shorter cut) 2/5lbs	case	5</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>5 32RIG1</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>